<commit_message>
a working POC of inventory search
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cgupt\Documents\Liquid Diamonds\Old Ubuntu Documents\Liquidibles\Business Development\Analysis\AI Model Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{690D7052-7620-4632-9494-8D61C31CEDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E22FF93-2377-4A9D-A7D6-19C97D5C85B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10880" yWindow="0" windowWidth="11150" windowHeight="13080" xr2:uid="{29114743-8AD3-43B2-8968-7F57D7D7F2BF}"/>
+    <workbookView xWindow="3680" yWindow="3680" windowWidth="28800" windowHeight="15370" xr2:uid="{29114743-8AD3-43B2-8968-7F57D7D7F2BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Questions</t>
   </si>
@@ -70,6 +71,15 @@
   </si>
   <si>
     <t>Item Ids of stones in Round | 1.00 - 1.19 | D | VS2 category?</t>
+  </si>
+  <si>
+    <t>What's the total value of my stock?</t>
+  </si>
+  <si>
+    <t>Which stone in my inventory has least price?</t>
+  </si>
+  <si>
+    <t>Which category has most number of stones?</t>
   </si>
 </sst>
 </file>
@@ -436,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7380347D-594F-4B29-88BD-09DB66DF743B}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,7 +457,7 @@
     <col min="1" max="1" width="39.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -468,8 +478,11 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -479,68 +492,119 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>